<commit_message>
added for pdf file in image modal
</commit_message>
<xml_diff>
--- a/stone-list/src/assets/StoneList.xlsx
+++ b/stone-list/src/assets/StoneList.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34">
   <si>
     <t>Name</t>
   </si>
@@ -28,6 +28,9 @@
     <t>Videos</t>
   </si>
   <si>
+    <t>Files</t>
+  </si>
+  <si>
     <t>Sapphire</t>
   </si>
   <si>
@@ -302,6 +305,64 @@
         <rFont val="Arial"/>
       </rPr>
       <t>[https://drive.google.com/file/d/1tST6Mu0bNJZRZV4utlJh13deM-gYRRSL/view?usp=drive_link,https://drive.google.com/file/d/13_NA1H8t85PFXONh5AN9Ti7RbbM3EKcE/view?usp=drive_link]</t>
+    </r>
+  </si>
+  <si>
+    <t>Ruby Necklace</t>
+  </si>
+  <si>
+    <t>Natural (33 pieces) some are Red &amp; some are Pigeon Blood color</t>
+  </si>
+  <si>
+    <t>USD - 4 millions</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="11"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>[https://drive.google.com/file/d/1wBiiQ9sF0-rWSixLS3qtCamImi_FIiKi/view?usp=drive_link]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="11"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>https://drive.google.com/file/d/1k9fM7cg01YITiitPDL6Jda50TLNYT0NO/view?usp=drive_link</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="11"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>[https://drive.google.com/file/d/1hl6d9iMoFpet0_Y8u9n6TG5qcMScUp57/view?usp=drive_link]</t>
     </r>
   </si>
 </sst>
@@ -421,7 +482,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -448,6 +509,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1501,13 +1565,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6667" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="6" width="12.6719" style="1" customWidth="1"/>
+    <col min="1" max="3" width="12.6719" style="1" customWidth="1"/>
+    <col min="4" max="4" width="27.3984" style="1" customWidth="1"/>
+    <col min="5" max="6" width="12.6719" style="1" customWidth="1"/>
     <col min="7" max="16384" width="12.6719" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1527,95 +1593,117 @@
       <c r="E1" t="s" s="2">
         <v>4</v>
       </c>
-      <c r="F1" s="2"/>
+      <c r="F1" t="s" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" ht="29.65" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" s="3"/>
     </row>
     <row r="3" ht="25.7" customHeight="1">
       <c r="A3" t="s" s="4">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s" s="5">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s" s="5">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s" s="5">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="7"/>
     </row>
     <row r="4" ht="25.7" customHeight="1">
       <c r="A4" t="s" s="4">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s" s="5">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s" s="5">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s" s="5">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s" s="8">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F4" s="7"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
       <c r="A5" t="s" s="4">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s" s="5">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s" s="5">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s" s="5">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s" s="5">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F5" s="6"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
       <c r="A6" t="s" s="4">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s" s="5">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s" s="5">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s" s="5">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E6" t="s" s="5">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F6" s="6"/>
+    </row>
+    <row r="7" ht="46.65" customHeight="1">
+      <c r="A7" t="s" s="4">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s" s="5">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s" s="5">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s" s="9">
+        <v>31</v>
+      </c>
+      <c r="E7" t="s" s="5">
+        <v>32</v>
+      </c>
+      <c r="F7" t="s" s="8">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1628,6 +1716,9 @@
     <hyperlink ref="E5" r:id="rId7" location="" tooltip="" display="[https://drive.google.com/file/d/1Qz87HBtMI1m3VPd8xet7MDFmfROFrDXh/view?usp=drive_link,https://drive.google.com/file/d/1bM8Eu8EWnR2-THYjZxy5s1vljDT_njFc/view?usp=drive_link]"/>
     <hyperlink ref="D6" r:id="rId8" location="" tooltip="" display="[https://drive.google.com/file/d/1QKl4YoyUcvjKQ1jHck51mCcWG7YoJLly/view?usp=drive_link]"/>
     <hyperlink ref="E6" r:id="rId9" location="" tooltip="" display="[https://drive.google.com/file/d/1tST6Mu0bNJZRZV4utlJh13deM-gYRRSL/view?usp=drive_link,https://drive.google.com/file/d/13_NA1H8t85PFXONh5AN9Ti7RbbM3EKcE/view?usp=drive_link]"/>
+    <hyperlink ref="D7" r:id="rId10" location="" tooltip="" display="[https://drive.google.com/file/d/1wBiiQ9sF0-rWSixLS3qtCamImi_FIiKi/view?usp=drive_link]"/>
+    <hyperlink ref="E7" r:id="rId11" location="" tooltip="" display="https://drive.google.com/file/d/1k9fM7cg01YITiitPDL6Jda50TLNYT0NO/view?usp=drive_link"/>
+    <hyperlink ref="F7" r:id="rId12" location="" tooltip="" display="[https://drive.google.com/file/d/1hl6d9iMoFpet0_Y8u9n6TG5qcMScUp57/view?usp=drive_link]"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>